<commit_message>
se implementa la una nueva funcion de borrar las url, y se coloca un nuevo dato para cuando se registra los almuerzos
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/reporte-almuerzos-empl.xlsx
+++ b/src/Views/assets/excel/reporte-almuerzos-empl.xlsx
@@ -9,15 +9,15 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$2:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$L$2</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Relacion de Solicitudes</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Bebida</t>
+  </si>
+  <si>
+    <t>Solicitud</t>
   </si>
 </sst>
 </file>
@@ -88,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -124,6 +127,15 @@
       <left style="thin">
         <color theme="1"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
       <right style="thin">
         <color theme="1"/>
       </right>
@@ -139,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -157,15 +169,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -717,7 +726,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -740,13 +749,13 @@
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
     <row r="2" s="1" customFormat="1">
@@ -783,7 +792,9 @@
       <c r="K2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
       <c r="E13" s="1"/>
@@ -816,10 +827,10 @@
       <c r="E22" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:K2"/>
+  <autoFilter ref="A2:L2"/>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="D1:L1"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
se coloca en el listado de la solicitud de los que soolicitaron dietas el tipo de pago
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/reporte-almuerzos-empl.xlsx
+++ b/src/Views/assets/excel/reporte-almuerzos-empl.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$L$2</definedName>
   </definedNames>
   <calcPr/>
@@ -52,7 +52,7 @@
     <t>Ensalada</t>
   </si>
   <si>
-    <t>Bebida</t>
+    <t xml:space="preserve">Tipo de Pago</t>
   </si>
   <si>
     <t>Solicitud</t>
@@ -127,10 +127,10 @@
       <left style="thin">
         <color theme="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -726,7 +726,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
       <selection activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -738,7 +738,8 @@
     <col customWidth="1" min="4" max="4" style="1" width="24.7109375"/>
     <col customWidth="1" min="5" max="9" style="1" width="17.28125"/>
     <col customWidth="1" min="10" max="10" style="1" width="34.57421875"/>
-    <col customWidth="1" min="11" max="12" style="1" width="17.28125"/>
+    <col customWidth="1" min="11" max="11" style="1" width="24.8515625"/>
+    <col customWidth="1" min="12" max="12" style="1" width="17.28125"/>
     <col min="13" max="16384" style="1" width="11.421875"/>
   </cols>
   <sheetData>

</xml_diff>